<commit_message>
run cucumber test runner from testng.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/Tdata.xlsx
+++ b/src/test/resources/Tdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerinjames/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerinjames/Desktop/JavaProblems/AmazonHybridProject/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FBD9AE-7463-344E-86F7-65543F20C7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D250D9-F5DE-C747-83D5-4CBD3CAD247D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{6DD23FBF-41C9-2D46-B49E-B053C53E83A7}"/>
   </bookViews>
@@ -35,12 +35,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Password</t>
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>jerinjamesm@gmail.com</t>
   </si>
   <si>
     <t>Girlboss27*</t>
@@ -50,10 +53,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -76,13 +87,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,7 +412,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -415,14 +429,17 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>919392118138</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EF47811B-6473-FF44-BF1E-4AEA1F68FD00}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>